<commit_message>
Intermediate check-in for using geographic region
</commit_message>
<xml_diff>
--- a/app/config/tables/geographic_regions/forms/geographic_regions/geographic_regions.xlsx
+++ b/app/config/tables/geographic_regions/forms/geographic_regions/geographic_regions.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
   <si>
     <t>comments</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>Ingrese el grupo privilegiado:</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -888,7 +891,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1080,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Remove additional / at end of geoRegion name
</commit_message>
<xml_diff>
--- a/app/config/tables/geographic_regions/forms/geographic_regions/geographic_regions.xlsx
+++ b/app/config/tables/geographic_regions/forms/geographic_regions/geographic_regions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26390" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26390" windowHeight="13940" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="7" r:id="rId1"/>
@@ -386,6 +386,21 @@
     <t>calculates.getDisplayName()</t>
   </si>
   <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>display.text</t>
+  </si>
+  <si>
+    <t>do section survey</t>
+  </si>
+  <si>
+    <t>goto _finalize</t>
+  </si>
+  <si>
+    <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
+  </si>
+  <si>
     <t>(function() {
   var name = '';
   var maxLevel = 5;
@@ -396,23 +411,9 @@
    if (i &lt; maxLevel) { name += '/'; }
     }
   } 
+  if (name.length &gt; 0 &amp;&amp; name.charAt(name.length - 1) === '/') {name = name.substr(0, name.length - 1)}
   return name;
 })()</t>
-  </si>
-  <si>
-    <t>instance_name</t>
-  </si>
-  <si>
-    <t>display.text</t>
-  </si>
-  <si>
-    <t>do section survey</t>
-  </si>
-  <si>
-    <t>goto _finalize</t>
-  </si>
-  <si>
-    <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
   </si>
 </sst>
 </file>
@@ -963,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -982,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>0</v>
@@ -990,19 +991,19 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1387,14 +1388,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="31.75" customWidth="1"/>
+    <col min="2" max="2" width="85.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1405,12 +1406,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="201.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="217" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1828,7 +1829,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>112</v>

</xml_diff>